<commit_message>
Add first batch of munge scripts
</commit_message>
<xml_diff>
--- a/data/states.xlsx
+++ b/data/states.xlsx
@@ -29,165 +29,84 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
-    <t>AC</t>
-  </si>
-  <si>
     <t>Acre</t>
   </si>
   <si>
-    <t>AL</t>
-  </si>
-  <si>
     <t>Alagoas</t>
   </si>
   <si>
-    <t>AM</t>
-  </si>
-  <si>
     <t>Amazonas</t>
   </si>
   <si>
-    <t>AP</t>
-  </si>
-  <si>
     <t>Amapá</t>
   </si>
   <si>
-    <t>BA</t>
-  </si>
-  <si>
     <t>Bahia</t>
   </si>
   <si>
-    <t>CE</t>
-  </si>
-  <si>
     <t>Ceará</t>
   </si>
   <si>
-    <t>DF</t>
-  </si>
-  <si>
     <t>Distrito Federal</t>
   </si>
   <si>
-    <t>ES</t>
-  </si>
-  <si>
     <t>Espírito Santo</t>
   </si>
   <si>
-    <t>GO</t>
-  </si>
-  <si>
     <t>Goiás</t>
   </si>
   <si>
-    <t>MA</t>
-  </si>
-  <si>
     <t>Maranhão</t>
   </si>
   <si>
-    <t>MG</t>
-  </si>
-  <si>
     <t>Minas Gerais</t>
   </si>
   <si>
-    <t>MS</t>
-  </si>
-  <si>
     <t>Mato Grosso do Sul</t>
   </si>
   <si>
-    <t>MT</t>
-  </si>
-  <si>
     <t>Mato Grosso</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
     <t>Pará</t>
   </si>
   <si>
-    <t>PB</t>
-  </si>
-  <si>
     <t>Paraíba</t>
   </si>
   <si>
-    <t>PE</t>
-  </si>
-  <si>
     <t>Pernambuco</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>Piauí</t>
   </si>
   <si>
-    <t>PR</t>
-  </si>
-  <si>
     <t>Paraná</t>
   </si>
   <si>
-    <t>RJ</t>
-  </si>
-  <si>
     <t>Rio de Janeiro</t>
   </si>
   <si>
-    <t>RN</t>
-  </si>
-  <si>
     <t>Rio Grande do Norte</t>
   </si>
   <si>
-    <t>RO</t>
-  </si>
-  <si>
     <t>Rondônia</t>
   </si>
   <si>
-    <t>RR</t>
-  </si>
-  <si>
     <t>Roraima</t>
   </si>
   <si>
-    <t>RS</t>
-  </si>
-  <si>
     <t>Rio Grande do Sul</t>
   </si>
   <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t>Santa Catarina</t>
   </si>
   <si>
-    <t>SE</t>
-  </si>
-  <si>
     <t>Sergipe</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>São Paulo</t>
   </si>
   <si>
-    <t>TO</t>
-  </si>
-  <si>
     <t>Tocantins</t>
   </si>
   <si>
@@ -195,6 +114,87 @@
   </si>
   <si>
     <t>estado</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>al</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>ap</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
+  <si>
+    <t>ce</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>go</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>pb</t>
+  </si>
+  <si>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>rj</t>
+  </si>
+  <si>
+    <t>rn</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>rr</t>
+  </si>
+  <si>
+    <t>rs</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>se</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>to</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,226 +522,226 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>